<commit_message>
Update timer diagram and notes after comments from Phillip
</commit_message>
<xml_diff>
--- a/Ch4_IOTimers/TimerCalculations.xlsx
+++ b/Ch4_IOTimers/TimerCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleci\work\oreilly\git\Ch4_IOTimers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDED267-D0E4-4A5C-9B4F-854D574C89C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91676DBC-9011-4D84-A958-7C10795494F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{268E9A45-B72B-4E46-8DD5-3BA3DB6729FB}"/>
   </bookViews>
@@ -574,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638DD760-803F-49CE-B964-3F0AC635183B}">
-  <dimension ref="A2:K148"/>
+  <dimension ref="A2:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,12 +700,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="O18">
+        <v>235294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -716,7 +719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -728,7 +731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -739,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -750,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -762,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>7</v>
       </c>
@@ -770,7 +773,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>5</v>
       </c>
@@ -782,7 +785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -794,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -806,12 +809,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>2</v>
       </c>
@@ -822,7 +825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>2</v>
       </c>
@@ -834,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>21</v>
       </c>
@@ -845,15 +848,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <f>C35/(C36*C38)</f>
+        <v>922.72202998846592</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>15</v>
       </c>
@@ -864,12 +871,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -881,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>20</v>
       </c>
@@ -893,7 +900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>25</v>
       </c>
@@ -904,12 +911,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>27</v>
       </c>
@@ -923,7 +930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>922</v>
       </c>
@@ -939,8 +946,12 @@
         <f>100*(ABS(D47-$C$38)/$C$38)</f>
         <v>7.8311278575489668E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H47">
+        <f>($C$35/$C$38)/B47</f>
+        <v>255.1996937603675</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B48">
         <f>B47+1</f>
         <v>923</v>

</xml_diff>

<commit_message>
Clarification updates to timer calculator
</commit_message>
<xml_diff>
--- a/Ch4_IOTimers/TimerCalculations.xlsx
+++ b/Ch4_IOTimers/TimerCalculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleci\work\oreilly\git\Ch4_IOTimers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91676DBC-9011-4D84-A958-7C10795494F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC5716D-774C-4140-BD99-D135A92211B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{268E9A45-B72B-4E46-8DD5-3BA3DB6729FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>prescaler = clockIn / (compare * timerFrequency)</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>max value, 10-bit register</t>
+  </si>
+  <si>
+    <t>Input data</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Key:</t>
   </si>
 </sst>
 </file>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638DD760-803F-49CE-B964-3F0AC635183B}">
-  <dimension ref="A2:O148"/>
+  <dimension ref="A1:K148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,15 +596,26 @@
     <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -700,15 +720,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O18">
-        <v>235294</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -719,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -731,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -742,7 +759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -753,7 +770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -765,7 +782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>7</v>
       </c>
@@ -773,7 +790,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>5</v>
       </c>
@@ -785,7 +802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>16</v>
       </c>
@@ -797,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -809,12 +826,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>2</v>
       </c>
@@ -825,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>2</v>
       </c>
@@ -837,7 +854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>21</v>
       </c>
@@ -848,19 +865,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
       </c>
-      <c r="G37">
-        <f>C35/(C36*C38)</f>
-        <v>922.72202998846592</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>15</v>
       </c>
@@ -871,12 +884,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -888,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>20</v>
       </c>
@@ -900,7 +913,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>25</v>
       </c>
@@ -911,12 +924,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>27</v>
       </c>
@@ -930,7 +943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>922</v>
       </c>
@@ -946,12 +959,8 @@
         <f>100*(ABS(D47-$C$38)/$C$38)</f>
         <v>7.8311278575489668E-2</v>
       </c>
-      <c r="H47">
-        <f>($C$35/$C$38)/B47</f>
-        <v>255.1996937603675</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B48">
         <f>B47+1</f>
         <v>923</v>

</xml_diff>